<commit_message>
began script to block study/test orders
</commit_message>
<xml_diff>
--- a/cfs_allExpts/afc_shortStudyLists/stimPairings.xlsx
+++ b/cfs_allExpts/afc_shortStudyLists/stimPairings.xlsx
@@ -11,10 +11,6 @@
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -356,8 +352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="B198" sqref="B198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,7 +381,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>199</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -412,7 +408,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>195</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -538,7 +534,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>198</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -997,7 +993,7 @@
         <v>71</v>
       </c>
       <c r="B71">
-        <v>200</v>
+        <v>20</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1744,7 +1740,7 @@
         <v>154</v>
       </c>
       <c r="B154">
-        <v>193</v>
+        <v>176</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -1942,7 +1938,7 @@
         <v>176</v>
       </c>
       <c r="B176">
-        <v>196</v>
+        <v>154</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -2095,7 +2091,7 @@
         <v>193</v>
       </c>
       <c r="B193">
-        <v>154</v>
+        <v>198</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
@@ -2113,7 +2109,7 @@
         <v>195</v>
       </c>
       <c r="B195">
-        <v>6</v>
+        <v>199</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
@@ -2122,7 +2118,7 @@
         <v>196</v>
       </c>
       <c r="B196">
-        <v>176</v>
+        <v>200</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
@@ -2140,7 +2136,7 @@
         <v>198</v>
       </c>
       <c r="B198">
-        <v>20</v>
+        <v>193</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
@@ -2149,7 +2145,7 @@
         <v>199</v>
       </c>
       <c r="B199">
-        <v>3</v>
+        <v>195</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
@@ -2158,7 +2154,7 @@
         <v>200</v>
       </c>
       <c r="B200">
-        <v>71</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>